<commit_message>
fix arima models and add sarima
</commit_message>
<xml_diff>
--- a/coverage_80.xlsx
+++ b/coverage_80.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,19 +533,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.806629834254144</v>
+        <v>0.8121546961325971</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8695652173913041</v>
+        <v>0.8641304347826091</v>
       </c>
       <c r="D7" t="n">
         <v>0.8532608695652171</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8516483516483521</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8454172366621071</v>
+        <v>0.846785225718194</v>
       </c>
     </row>
     <row r="8">
@@ -555,16 +555,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8232044198895031</v>
+        <v>0.8011049723756911</v>
       </c>
       <c r="C8" t="n">
+        <v>0.8804347826086961</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.885869565217391</v>
       </c>
-      <c r="D8" t="n">
-        <v>0.875</v>
-      </c>
       <c r="E8" t="n">
-        <v>0.862637362637363</v>
+        <v>0.8791208791208791</v>
       </c>
       <c r="F8" t="n">
         <v>0.8618331053351571</v>
@@ -577,19 +577,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.81767955801105</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.8695652173913041</v>
+        <v>0.6740331491712711</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0.7391304347826091</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7934782608695651</v>
+        <v>0.641304347826087</v>
       </c>
       <c r="E9" t="n">
-        <v>0.807692307692308</v>
+        <v>0.6538461538461541</v>
       </c>
       <c r="F9" t="n">
-        <v>0.822161422708618</v>
+        <v>0.6771545827633381</v>
       </c>
     </row>
     <row r="10">
@@ -598,20 +598,20 @@
           <t>TBATS_rf</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>0.6132596685082871</v>
+      <c r="B10" s="2" t="n">
+        <v>0.629834254143646</v>
       </c>
       <c r="C10" t="n">
         <v>0.8152173913043481</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5978260869565221</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.467032967032967</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.6238030095759231</v>
+        <v>0.630434782608696</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.472527472527472</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.6374829001367991</v>
       </c>
     </row>
     <row r="11">
@@ -624,16 +624,16 @@
         <v>0.81767955801105</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8804347826086961</v>
+        <v>0.885869565217391</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8804347826086961</v>
+        <v>0.896739130434783</v>
       </c>
       <c r="E11" t="n">
         <v>0.868131868131868</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8618331053351571</v>
+        <v>0.867305061559507</v>
       </c>
     </row>
     <row r="12">
@@ -643,19 +643,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.558011049723757</v>
+        <v>0.906077348066298</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3097826086956521</v>
+        <v>0.777173913043478</v>
       </c>
       <c r="D12" t="n">
-        <v>0.445652173913043</v>
+        <v>0.755434782608696</v>
       </c>
       <c r="E12" t="n">
-        <v>0.208791208791209</v>
+        <v>0.868131868131868</v>
       </c>
       <c r="F12" t="n">
-        <v>0.380300957592339</v>
+        <v>0.826265389876881</v>
       </c>
     </row>
     <row r="13">
@@ -665,19 +665,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.856353591160221</v>
+        <v>0.751381215469613</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6739130434782611</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.8586956521739131</v>
+        <v>0.75</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.478260869565217</v>
       </c>
       <c r="E13" t="n">
-        <v>0.681318681318681</v>
+        <v>0.5934065934065941</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7674418604651161</v>
+        <v>0.642954856361149</v>
       </c>
     </row>
     <row r="14">
@@ -687,19 +687,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.878453038674033</v>
+        <v>0.8674033149171271</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8532608695652171</v>
+        <v>0.875</v>
       </c>
       <c r="D14" t="n">
-        <v>0.826086956521739</v>
+        <v>0.8478260869565221</v>
       </c>
       <c r="E14" t="n">
         <v>0.8186813186813191</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8440492476060191</v>
+        <v>0.8522571819425441</v>
       </c>
     </row>
     <row r="15">
@@ -708,20 +708,20 @@
           <t>arima1_1_2</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n">
-        <v>0.552486187845304</v>
+      <c r="B15" t="n">
+        <v>0.8397790055248621</v>
       </c>
       <c r="C15" t="n">
-        <v>0.260869565217391</v>
+        <v>0.8423913043478261</v>
       </c>
       <c r="D15" t="n">
-        <v>0.391304347826087</v>
+        <v>0.8804347826086961</v>
       </c>
       <c r="E15" t="n">
-        <v>0.252747252747253</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="F15" t="n">
-        <v>0.363885088919289</v>
+        <v>0.854993160054719</v>
       </c>
     </row>
     <row r="16">
@@ -731,19 +731,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.5966850828729281</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>0.190217391304348</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>0.184782608695652</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>0.148351648351648</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>0.27906976744186</v>
+        <v>0.8397790055248621</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8641304347826091</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.859097127222982</v>
       </c>
     </row>
     <row r="17">
@@ -753,19 +753,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.558011049723757</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.244565217391304</v>
+        <v>0.75</v>
       </c>
       <c r="D17" t="n">
-        <v>0.358695652173913</v>
+        <v>0.8423913043478261</v>
       </c>
       <c r="E17" t="n">
-        <v>0.230769230769231</v>
+        <v>0.967032967032967</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3474692202462381</v>
+        <v>0.8891928864569081</v>
       </c>
     </row>
     <row r="18">
@@ -775,19 +775,63 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.558011049723757</v>
+        <v>0.9005524861878451</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3097826086956521</v>
+        <v>0.777173913043478</v>
       </c>
       <c r="D18" t="n">
-        <v>0.445652173913043</v>
+        <v>0.755434782608696</v>
       </c>
       <c r="E18" t="n">
-        <v>0.208791208791209</v>
+        <v>0.868131868131868</v>
       </c>
       <c r="F18" t="n">
-        <v>0.380300957592339</v>
+        <v>0.8248974008207931</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>arima1_0_2</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.9668508287292821</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.771739130434783</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.8358413132694941</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>sarima212_001</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.755434782608696</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.8423913043478261</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.967032967032967</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.8358413132694941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>